<commit_message>
update : changes in prompt
</commit_message>
<xml_diff>
--- a/PROJECT_features.xlsx
+++ b/PROJECT_features.xlsx
@@ -418,54 +418,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":1800,"ease_of_use":4.2,"features":4.5,"design":4.3,"support":4}</v>
+        <v>{"Total_reviews":2500,"Ease_of_use":4.5,"Features":4.7,"Design":4.2,"Support":4}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":true,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":true,"Cozyroc SSIS+ Suite":false,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other_available_integrations":"Hundreds of integrations available through the ServiceNow store"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Essential","Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on usage and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":true,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":true,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In-person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"ServiceNow","year_founded":2004,"country":"United States"}</v>
+        <v>{"Company_name":"ServiceNow","Year_founded":2004,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","IT Operations Management","Service Level Management","Reporting and Analytics","Automation","AI and Machine Learning","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","IT Asset Management","Workflow Automation","Reporting and Analytics","Cloud Management","Security Management","Customer Service Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -484,54 +484,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":300,"ease_of_use":3.7,"features":4.2,"design":3.5,"support":3.8}</v>
+        <v>{"Total_reviews":600,"Ease_of_use":3.8,"Features":4.2,"Design":3.5,"Support":3.7}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Standard","Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"BMC Software","year_founded":1980,"country":"United States"}</v>
+        <v>{"Company_name":"BMC Software","Year_founded":1980,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","IT Operations Management","Service Level Management","Reporting and Analytics","Automation","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Service Level Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -550,54 +550,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":400,"ease_of_use":3.9,"features":4.1,"design":3.7,"support":3.8}</v>
+        <v>{"Total_reviews":600,"Ease_of_use":4,"Features":4.2,"Design":3.9,"Support":3.8}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Standard","Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"Ivanti","year_founded":1994,"country":"United States"}</v>
+        <v>{"Company_name":"Ivanti","Year_founded":1994,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","IT Operations Management","Service Level Management","Reporting and Analytics","Automation","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Endpoint Management","Unified Endpoint Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -616,54 +616,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":200,"ease_of_use":3.8,"features":4,"design":3.6,"support":3.7}</v>
+        <v>{"Total_reviews":400,"Ease_of_use":4,"Features":4.1,"Design":3.7,"Support":3.9}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Standard","Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"EV Technologies","year_founded":2000,"country":"United Kingdom"}</v>
+        <v>{"Company_name":"EV Technologies","Year_founded":1996,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","IT Operations Management","Service Level Management","Reporting and Analytics","Automation","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Service Level Management","ITIL Process Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -682,54 +682,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":400,"ease_of_use":4.1,"features":4,"design":3.8,"support":3.9}</v>
+        <v>{"Total_reviews":900,"Ease_of_use":4.1,"Features":3.9,"Design":3.7,"Support":3.6}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"SolarWinds","year_founded":1999,"country":"United States"}</v>
+        <v>{"Company_name":"SolarWinds","Year_founded":1999,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","Reporting and Analytics","Automation","Integration with other tools"]</v>
+        <v>["Incident Management","Knowledge Management","Request Management","Workflow Automation","Reporting and Analytics","Self-service Portal","Email Ticketing"]</v>
       </c>
     </row>
   </sheetData>
@@ -748,54 +748,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":300,"ease_of_use":4,"features":4.2,"design":3.9,"support":3.8}</v>
+        <v>{"Total_reviews":700,"Ease_of_use":4.2,"Features":4,"Design":3.8,"Support":3.9}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Standard","Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"TeamDynamix","year_founded":2001,"country":"United States"}</v>
+        <v>{"Company_name":"TeamDynamix","Year_founded":2001,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","IT Operations Management","Service Level Management","Reporting and Analytics","Automation","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Project Management Integration"]</v>
       </c>
     </row>
   </sheetData>
@@ -814,54 +814,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":200,"ease_of_use":4,"features":4.1,"design":3.8,"support":3.9}</v>
+        <v>{"Total_reviews":500,"Ease_of_use":4.3,"Features":4.1,"Design":4,"Support":4}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Standard","Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"InvGate","year_founded":2001,"country":"Spain"}</v>
+        <v>{"Company_name":"InvGate","Year_founded":2009,"Country":"Argentina"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","IT Operations Management","Service Level Management","Reporting and Analytics","Automation","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Self-service Portal","ITIL Process Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -880,54 +880,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":700,"ease_of_use":4.1,"features":4,"design":3.8,"support":3.9}</v>
+        <v>{"Total_reviews":1500,"Ease_of_use":4.2,"Features":4,"Design":3.8,"Support":3.7}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In-person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"SolarWinds","year_founded":1999,"country":"United States"}</v>
+        <v>{"Company_name":"SolarWinds","Year_founded":1999,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","Reporting and Analytics","Automation","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","Workflow Automation","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -946,54 +946,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":600,"ease_of_use":4,"features":4.2,"design":3.7,"support":3.8}</v>
+        <v>{"Total_reviews":1200,"Ease_of_use":4,"Features":4.2,"Design":3.5,"Support":3.8}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In-person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"ManageEngine","year_founded":2001,"country":"India"}</v>
+        <v>{"Company_name":"ManageEngine","Year_founded":2001,"Country":"India"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","Reporting and Analytics","Automation","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -1012,54 +1012,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":500,"ease_of_use":4,"features":4.1,"design":3.9,"support":3.7}</v>
+        <v>{"Total_reviews":800,"Ease_of_use":4.3,"Features":4.1,"Design":3.9,"Support":4}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Standard","Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In-person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"TOPdesk","year_founded":1993,"country":"Netherlands"}</v>
+        <v>{"Company_name":"TOPdesk","Year_founded":1993,"Country":"Netherlands"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","Reporting and Analytics","Automation","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -1078,54 +1078,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":300,"ease_of_use":3.8,"features":4.3,"design":3.6,"support":3.9}</v>
+        <v>{"Total_reviews":500,"Ease_of_use":4,"Features":4.3,"Design":3.8,"Support":3.7}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Standard","Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In-person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"SymphonyAI","year_founded":2017,"country":"United States"}</v>
+        <v>{"Company_name":"SymphonyAI","Year_founded":2017,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","IT Operations Management","Service Level Management","Reporting and Analytics","Automation","AI and Machine Learning","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","AI-powered automation","Predictive analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -1144,54 +1144,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":1500,"ease_of_use":4.3,"features":4.4,"design":4.1,"support":3.9}</v>
+        <v>{"Total_reviews":2000,"Ease_of_use":4.2,"Features":4.4,"Design":3.9,"Support":3.8}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":true,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":true,"Cozyroc SSIS+ Suite":false,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other_available_integrations":"Hundreds of integrations available through the Atlassian Marketplace"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Standard","Premium"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In-person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"Atlassian","year_founded":2002,"country":"Australia"}</v>
+        <v>{"Company_name":"Atlassian","Year_founded":2002,"Country":"Australia"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","Reporting and Analytics","Automation","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","Workflow Automation","Reporting and Analytics","Project Management Integration","Agile Development Integration"]</v>
       </c>
     </row>
   </sheetData>
@@ -1210,54 +1210,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":400,"ease_of_use":3.9,"features":4.1,"design":3.7,"support":3.8}</v>
+        <v>{"Total_reviews":700,"Ease_of_use":4.1,"Features":4.3,"Design":3.7,"Support":3.9}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Standard","Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"Cherwell Software","year_founded":1997,"country":"United States"}</v>
+        <v>{"Company_name":"Cherwell Software","Year_founded":1997,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","IT Operations Management","Service Level Management","Reporting and Analytics","Automation","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -1276,54 +1276,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":1200,"ease_of_use":4.4,"features":4.3,"design":4.2,"support":4.1}</v>
+        <v>{"Total_reviews":1800,"Ease_of_use":4.5,"Features":4.3,"Design":4.1,"Support":4.2}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":true,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":true,"Cozyroc SSIS+ Suite":false,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other_available_integrations":"Hundreds of integrations available through the Freshworks Marketplace"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Blossom","Garden","Estate","Forest"],"free_version_availability":true,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":true,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"Freshworks","year_founded":2010,"country":"India"}</v>
+        <v>{"Company_name":"Freshworks","Year_founded":2010,"Country":"India"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","IT Operations Management","Service Level Management","Reporting and Analytics","Automation","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Customer Service Management","AI-powered automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1342,54 +1342,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":500,"ease_of_use":4.2,"features":4,"design":3.8,"support":3.9}</v>
+        <v>{"Total_reviews":1000,"Ease_of_use":4.2,"Features":4.1,"Design":3.8,"Support":4}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":true,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":["Standard","Professional","Enterprise"],"free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"SysAid Technologies","year_founded":2001,"country":"Israel"}</v>
+        <v>{"Company_name":"SysAid Technologies","Year_founded":1999,"Country":"Israel"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Fulfillment","IT Operations Management","Service Level Management","Reporting and Analytics","Automation","Workflow Management","Integration with other tools"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Remote Desktop Support","Self-service Portal"]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update : added overall rating to requirements in gmini prompt
</commit_message>
<xml_diff>
--- a/PROJECT_features.xlsx
+++ b/PROJECT_features.xlsx
@@ -418,54 +418,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":2500,"Ease_of_use":4.5,"Features":4.7,"Design":4.2,"Support":4}</v>
+        <v>{"total_reviews":1000,"ease_of_use":4.5,"features":4.7,"design":4.3,"support":4.2,"overall":4.6}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":true,"Cozyroc SSIS+ Suite":false,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other_available_integrations":"Hundreds of integrations available through the ServiceNow store"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":true,"BigID":true,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on usage and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":true,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":true,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In-person_training":true}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"ServiceNow","Year_founded":2004,"Country":"United States"}</v>
+        <v>{"company_name":"ServiceNow","year_founded":2004,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","IT Asset Management","Workflow Automation","Reporting and Analytics","Cloud Management","Security Management","Customer Service Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","IT Operations Management","Cloud Management","Security Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -484,54 +484,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":600,"Ease_of_use":3.8,"Features":4.2,"Design":3.5,"Support":3.7}</v>
+        <v>{"total_reviews":75,"ease_of_use":3.5,"features":3.6,"design":3.3,"support":3.4,"overall":3.5}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In_person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"BMC Software","Year_founded":1980,"Country":"United States"}</v>
+        <v>{"company_name":"BMC Software","year_founded":1980,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Service Level Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -550,54 +550,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":600,"Ease_of_use":4,"Features":4.2,"Design":3.9,"Support":3.8}</v>
+        <v>{"total_reviews":125,"ease_of_use":4,"features":3.8,"design":3.7,"support":3.6,"overall":3.8}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In_person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"Ivanti","Year_founded":1994,"Country":"United States"}</v>
+        <v>{"company_name":"Ivanti","year_founded":1994,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Endpoint Management","Unified Endpoint Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","IT Operations Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -616,54 +616,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":400,"Ease_of_use":4,"Features":4.1,"Design":3.7,"Support":3.9}</v>
+        <v>{"total_reviews":100,"ease_of_use":3.7,"features":3.6,"design":3.4,"support":3.5,"overall":3.6}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In_person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"EV Technologies","Year_founded":1996,"Country":"United States"}</v>
+        <v>{"company_name":"EV Technologies","year_founded":1998,"country":"United Kingdom"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Service Level Management","ITIL Process Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -682,54 +682,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":900,"Ease_of_use":4.1,"Features":3.9,"Design":3.7,"Support":3.6}</v>
+        <v>{"total_reviews":200,"ease_of_use":3.8,"features":3.6,"design":3.5,"support":3.7,"overall":3.7}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In_person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"SolarWinds","Year_founded":1999,"Country":"United States"}</v>
+        <v>{"company_name":"SolarWinds","year_founded":1999,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Knowledge Management","Request Management","Workflow Automation","Reporting and Analytics","Self-service Portal","Email Ticketing"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -748,54 +748,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":700,"Ease_of_use":4.2,"Features":4,"Design":3.8,"Support":3.9}</v>
+        <v>{"total_reviews":150,"ease_of_use":3.9,"features":3.7,"design":3.6,"support":3.8,"overall":3.8}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In_person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"TeamDynamix","Year_founded":2001,"Country":"United States"}</v>
+        <v>{"company_name":"TeamDynamix","year_founded":2001,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Project Management Integration"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","Project Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -814,54 +814,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":500,"Ease_of_use":4.3,"Features":4.1,"Design":4,"Support":4}</v>
+        <v>{"total_reviews":100,"ease_of_use":4,"features":3.8,"design":3.7,"support":3.9,"overall":3.9}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":true,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In_person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"InvGate","Year_founded":2009,"Country":"Argentina"}</v>
+        <v>{"company_name":"InvGate","year_founded":2005,"country":"Argentina"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Self-service Portal","ITIL Process Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","IT Operations Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -880,54 +880,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":1500,"Ease_of_use":4.2,"Features":4,"Design":3.8,"Support":3.7}</v>
+        <v>{"total_reviews":500,"ease_of_use":4.2,"features":4,"design":3.8,"support":4,"overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":true,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In-person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"SolarWinds","Year_founded":1999,"Country":"United States"}</v>
+        <v>{"company_name":"SolarWinds","year_founded":1999,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","Workflow Automation","Reporting and Analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -946,54 +946,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":1200,"Ease_of_use":4,"Features":4.2,"Design":3.5,"Support":3.8}</v>
+        <v>{"total_reviews":300,"ease_of_use":4,"features":3.8,"design":3.5,"support":3.7,"overall":3.9}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":true,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In-person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"ManageEngine","Year_founded":2001,"Country":"India"}</v>
+        <v>{"company_name":"ManageEngine","year_founded":1999,"country":"India"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -1012,54 +1012,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":800,"Ease_of_use":4.3,"Features":4.1,"Design":3.9,"Support":4}</v>
+        <v>{"total_reviews":200,"ease_of_use":4.1,"features":3.9,"design":3.7,"support":3.8,"overall":3.9}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In-person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"TOPdesk","Year_founded":1993,"Country":"Netherlands"}</v>
+        <v>{"company_name":"TOPdesk","year_founded":1993,"country":"Netherlands"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -1078,54 +1078,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":500,"Ease_of_use":4,"Features":4.3,"Design":3.8,"Support":3.7}</v>
+        <v>{"total_reviews":150,"ease_of_use":4.3,"features":4.5,"design":4,"support":3.9,"overall":4.2}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":true,"BigID":true,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":true,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In-person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"SymphonyAI","Year_founded":2017,"Country":"United States"}</v>
+        <v>{"company_name":"SymphonyAI","year_founded":2017,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","AI-powered automation","Predictive analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","IT Operations Management","Cloud Management","Security Management","AI-powered automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1144,54 +1144,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":2000,"Ease_of_use":4.2,"Features":4.4,"Design":3.9,"Support":3.8}</v>
+        <v>{"total_reviews":800,"ease_of_use":4.4,"features":4.3,"design":4,"support":4.1,"overall":4.3}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":true,"Cozyroc SSIS+ Suite":false,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other_available_integrations":"Hundreds of integrations available through the Atlassian Marketplace"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":true,"BigID":false,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In-person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"Atlassian","Year_founded":2002,"Country":"Australia"}</v>
+        <v>{"company_name":"Atlassian","year_founded":2002,"country":"Australia"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","Workflow Automation","Reporting and Analytics","Project Management Integration","Agile Development Integration"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","Project Management","Agile Development"]</v>
       </c>
     </row>
   </sheetData>
@@ -1210,54 +1210,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":700,"Ease_of_use":4.1,"Features":4.3,"Design":3.7,"Support":3.9}</v>
+        <v>{"total_reviews":100,"ease_of_use":3.8,"features":3.7,"design":3.5,"support":3.6,"overall":3.7}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":false,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":false,"In_person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"Cherwell Software","Year_founded":1997,"Country":"United States"}</v>
+        <v>{"company_name":"Cherwell Software","year_founded":2000,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
       </c>
     </row>
   </sheetData>
@@ -1276,54 +1276,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":1800,"Ease_of_use":4.5,"Features":4.3,"Design":4.1,"Support":4.2}</v>
+        <v>{"total_reviews":400,"ease_of_use":4.2,"features":4,"design":3.9,"support":4,"overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":true,"Cozyroc SSIS+ Suite":false,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other_available_integrations":"Hundreds of integrations available through the Freshworks Marketplace"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":true,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":true,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In_person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"Freshworks","Year_founded":2010,"Country":"India"}</v>
+        <v>{"company_name":"Freshworks","year_founded":2010,"country":"India"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Customer Service Management","AI-powered automation"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","IT Operations Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -1342,54 +1342,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_reviews":1000,"Ease_of_use":4.2,"Features":4.1,"Design":3.8,"Support":4}</v>
+        <v>{"total_reviews":250,"ease_of_use":3.9,"features":3.7,"design":3.6,"support":3.8,"overall":3.8}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_access":true,"Integrations":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":true,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other_available_integrations":"Limited integrations available"}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_tiers":"Multiple tiers based on users and features","Free_version_availability":false,"Free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":true,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_online_sessions":true,"In_person_training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_name":"SysAid Technologies","Year_founded":1999,"Country":"Israel"}</v>
+        <v>{"company_name":"SysAid Technologies","year_founded":1999,"country":"Israel"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Catalog","Request Management","IT Service Continuity Management","Workflow Automation","Reporting and Analytics","Remote Desktop Support","Self-service Portal"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","Remote Support"]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the openai features
</commit_message>
<xml_diff>
--- a/PROJECT_features.xlsx
+++ b/PROJECT_features.xlsx
@@ -418,54 +418,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":1000,"ease_of_use":4.5,"features":4.7,"design":4.3,"support":4.2,"overall":4.6}</v>
+        <v>{"Total_Reviews":1000,"Ease_of_Use":4.5,"Features":4.7,"Design":4.3,"Support":4.2,"Overall":4.6}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":true,"BigID":true,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":true,"Assess360":true,"BigID":true,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count, features, and platform","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":true,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":true,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":true,"In-Person_Training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"ServiceNow","year_founded":2004,"country":"United States"}</v>
+        <v>{"Company_Name":"ServiceNow","Year_Founded":2004,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","IT Operations Management","Cloud Management","Security Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","IT Operations Management","Cloud Management","Security Management","Workflow Automation","AI-powered Chatbot"]</v>
       </c>
     </row>
   </sheetData>
@@ -484,54 +484,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":75,"ease_of_use":3.5,"features":3.6,"design":3.3,"support":3.4,"overall":3.5}</v>
+        <v>{"Total_Reviews":150,"Ease_of_Use":3.7,"Features":3.9,"Design":3.5,"Support":3.8,"Overall":3.7}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"BMC Software","year_founded":1980,"country":"United States"}</v>
+        <v>{"Company_Name":"BMC Software","Year_Founded":1980,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","IT Operations Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -550,54 +550,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":125,"ease_of_use":4,"features":3.8,"design":3.7,"support":3.6,"overall":3.8}</v>
+        <v>{"Total_Reviews":250,"Ease_of_Use":4.2,"Features":4.3,"Design":4,"Support":4.1,"Overall":4.2}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":true,"In-Person_Training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"Ivanti","year_founded":1994,"country":"United States"}</v>
+        <v>{"Company_Name":"Ivanti","Year_Founded":1994,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","IT Operations Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","Unified Endpoint Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -616,54 +616,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":100,"ease_of_use":3.7,"features":3.6,"design":3.4,"support":3.5,"overall":3.6}</v>
+        <v>{"Total_Reviews":100,"Ease_of_Use":3.9,"Features":4.1,"Design":3.7,"Support":3.9,"Overall":3.9}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"EV Technologies","year_founded":1998,"country":"United Kingdom"}</v>
+        <v>{"Company_Name":"EV Technologies","Year_Founded":1996,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -682,54 +682,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":200,"ease_of_use":3.8,"features":3.6,"design":3.5,"support":3.7,"overall":3.7}</v>
+        <v>{"Total_Reviews":200,"Ease_of_Use":4.1,"Features":3.9,"Design":3.8,"Support":3.9,"Overall":3.9}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"SolarWinds","year_founded":1999,"country":"United States"}</v>
+        <v>{"Company_Name":"SolarWinds","Year_Founded":1999,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
+        <v>["Incident Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -748,54 +748,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":150,"ease_of_use":3.9,"features":3.7,"design":3.6,"support":3.8,"overall":3.8}</v>
+        <v>{"Total_Reviews":150,"Ease_of_Use":4,"Features":4.2,"Design":3.9,"Support":4,"Overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"TeamDynamix","year_founded":2001,"country":"United States"}</v>
+        <v>{"Company_Name":"TeamDynamix","Year_Founded":2001,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","Project Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","Project Management Integration"]</v>
       </c>
     </row>
   </sheetData>
@@ -814,54 +814,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":100,"ease_of_use":4,"features":3.8,"design":3.7,"support":3.9,"overall":3.9}</v>
+        <v>{"Total_Reviews":200,"Ease_of_Use":4.3,"Features":4.4,"Design":4.1,"Support":4.2,"Overall":4.3}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":true,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"InvGate","year_founded":2005,"country":"Argentina"}</v>
+        <v>{"Company_Name":"InvGate","Year_Founded":2009,"Country":"Argentina"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","IT Operations Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -880,54 +880,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":500,"ease_of_use":4.2,"features":4,"design":3.8,"support":4,"overall":4.1}</v>
+        <v>{"Total_Reviews":500,"Ease_of_Use":4.2,"Features":4.1,"Design":3.9,"Support":4,"Overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":true,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"SolarWinds","year_founded":1999,"country":"United States"}</v>
+        <v>{"Company_Name":"SolarWinds","Year_Founded":1999,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -946,54 +946,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":300,"ease_of_use":4,"features":3.8,"design":3.5,"support":3.7,"overall":3.9}</v>
+        <v>{"Total_Reviews":400,"Ease_of_Use":4,"Features":4.2,"Design":3.8,"Support":3.9,"Overall":4}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":true,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"ManageEngine","year_founded":1999,"country":"India"}</v>
+        <v>{"Company_Name":"ManageEngine","Year_Founded":2001,"Country":"India"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1012,54 +1012,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":200,"ease_of_use":4.1,"features":3.9,"design":3.7,"support":3.8,"overall":3.9}</v>
+        <v>{"Total_Reviews":300,"Ease_of_Use":4.1,"Features":4.3,"Design":3.9,"Support":4,"Overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"TOPdesk","year_founded":1993,"country":"Netherlands"}</v>
+        <v>{"Company_Name":"TOPdesk","Year_Founded":1993,"Country":"Netherlands"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1078,54 +1078,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":150,"ease_of_use":4.3,"features":4.5,"design":4,"support":3.9,"overall":4.2}</v>
+        <v>{"Total_Reviews":200,"Ease_of_Use":4.3,"Features":4.5,"Design":4.1,"Support":4.2,"Overall":4.4}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":true,"BigID":true,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":true,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":true,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":true,"In-Person_Training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"SymphonyAI","year_founded":2017,"country":"United States"}</v>
+        <v>{"Company_Name":"SymphonyAI","Year_Founded":2017,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","IT Operations Management","Cloud Management","Security Management","AI-powered automation"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","IT Operations Management","AI-powered Chatbot","Predictive Analytics","Automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1144,54 +1144,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":800,"ease_of_use":4.4,"features":4.3,"design":4,"support":4.1,"overall":4.3}</v>
+        <v>{"Total_Reviews":1000,"Ease_of_Use":4.2,"Features":4.4,"Design":4,"Support":4.1,"Overall":4.3}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":true,"BigID":false,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":true,"In-Person_Training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"Atlassian","year_founded":2002,"country":"Australia"}</v>
+        <v>{"Company_Name":"Atlassian","Year_Founded":2002,"Country":"Australia"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","Project Management","Agile Development"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","Project Management Integration"]</v>
       </c>
     </row>
   </sheetData>
@@ -1210,54 +1210,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":100,"ease_of_use":3.8,"features":3.7,"design":3.5,"support":3.6,"overall":3.7}</v>
+        <v>{"Total_Reviews":200,"Ease_of_Use":3.8,"Features":4,"Design":3.7,"Support":3.9,"Overall":3.8}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":true}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"Cherwell Software","year_founded":2000,"country":"United States"}</v>
+        <v>{"Company_Name":"Cherwell Software","Year_Founded":1997,"Country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1276,54 +1276,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":400,"ease_of_use":4.2,"features":4,"design":3.9,"support":4,"overall":4.1}</v>
+        <v>{"Total_Reviews":600,"Ease_of_Use":4.4,"Features":4.3,"Design":4.2,"Support":4.1,"Overall":4.3}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":true,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"Freshworks","year_founded":2010,"country":"India"}</v>
+        <v>{"Company_Name":"Freshworks","Year_Founded":2010,"Country":"India"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","IT Operations Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","AI-powered Chatbot"]</v>
       </c>
     </row>
   </sheetData>
@@ -1342,54 +1342,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ratings</v>
+        <v>Ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>api_and_integration_support</v>
+        <v>API_and_Integration_Support</v>
       </c>
       <c r="C1" t="str">
-        <v>pricing_details</v>
+        <v>Pricing_Details</v>
       </c>
       <c r="D1" t="str">
-        <v>deployment_support</v>
+        <v>Deployment_Support</v>
       </c>
       <c r="E1" t="str">
-        <v>customer_support_options</v>
+        <v>Customer_Support_Options</v>
       </c>
       <c r="F1" t="str">
-        <v>training_platforms</v>
+        <v>Training_Platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>vendor_details</v>
+        <v>Vendor_Details</v>
       </c>
       <c r="H1" t="str">
-        <v>features</v>
+        <v>List_of_Features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":250,"ease_of_use":3.9,"features":3.7,"design":3.6,"support":3.8,"overall":3.8}</v>
+        <v>{"Total_Reviews":300,"Ease_of_Use":4,"Features":4.1,"Design":3.8,"Support":4,"Overall":4}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact vendor for pricing","free_version_availability":true,"free_trial_availability":true}</v>
+        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"documentation":true,"webinars":true,"live_online_sessions":false,"in_person_training":false}</v>
+        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"SysAid Technologies","year_founded":1999,"country":"Israel"}</v>
+        <v>{"Company_Name":"SysAid Technologies","Year_Founded":1999,"Country":"Israel"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Asset Management","Knowledge Management","Service Catalog","Request Management","Service Level Management","Reporting and Analytics","Remote Support"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","Remote Desktop Support"]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Top 3 tools details
</commit_message>
<xml_diff>
--- a/PROJECT_features.xlsx
+++ b/PROJECT_features.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="ServiceNow IT Service Managemen" sheetId="1" r:id="rId1"/>
+    <sheet name="ServiceNow ITSM" sheetId="1" r:id="rId1"/>
     <sheet name="SolarWinds Service Desk" sheetId="2" r:id="rId2"/>
     <sheet name="ServiceDesk Plus" sheetId="3" r:id="rId3"/>
     <sheet name="TOPdesk" sheetId="4" r:id="rId4"/>
@@ -418,54 +418,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":1000,"Ease_of_Use":4.5,"Features":4.7,"Design":4.3,"Support":4.2,"Overall":4.6}</v>
+        <v>{"total_reviews":1000,"ease_of_use":4.5,"features":4.7,"design":4.3,"support":4.2,"overall":4.6}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":true,"Assess360":true,"BigID":true,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":true,"BigID":true,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other available integrations":"Numerous integrations with other popular business applications"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count, features, and platform","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Multiple tiers based on user count and features","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":true,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":true,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":true,"In-Person_Training":true}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"ServiceNow","Year_Founded":2004,"Country":"United States"}</v>
+        <v>{"company_name":"ServiceNow","year_founded":2004,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","IT Operations Management","Cloud Management","Security Management","Workflow Automation","AI-powered Chatbot"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Automation","Workflow Management","AI-powered insights"]</v>
       </c>
     </row>
   </sheetData>
@@ -484,54 +484,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":150,"Ease_of_Use":3.7,"Features":3.9,"Design":3.5,"Support":3.8,"Overall":3.7}</v>
+        <v>{"total_reviews":300,"ease_of_use":4,"features":4.2,"design":3.8,"support":3.9,"overall":4}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular IT management and business applications"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Contact sales for pricing information","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"BMC Software","Year_Founded":1980,"Country":"United States"}</v>
+        <v>{"company_name":"BMC Software","year_founded":1980,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","IT Operations Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -550,54 +550,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":250,"Ease_of_Use":4.2,"Features":4.3,"Design":4,"Support":4.1,"Overall":4.2}</v>
+        <v>{"total_reviews":200,"ease_of_use":4.1,"features":4.3,"design":3.9,"support":3.8,"overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular IT management and security tools"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Contact sales for pricing information","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":true,"In-Person_Training":true}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"Ivanti","Year_Founded":1994,"Country":"United States"}</v>
+        <v>{"company_name":"Ivanti","year_founded":1994,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","Unified Endpoint Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","AI-powered automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -616,54 +616,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":100,"Ease_of_Use":3.9,"Features":4.1,"Design":3.7,"Support":3.9,"Overall":3.9}</v>
+        <v>{"total_reviews":100,"ease_of_use":4,"features":4.1,"design":3.8,"support":3.9,"overall":4}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular IT management tools"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Contact sales for pricing information","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"EV Technologies","Year_Founded":1996,"Country":"United States"}</v>
+        <v>{"company_name":"EV Technologies","year_founded":1998,"country":"United Kingdom"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -682,54 +682,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":200,"Ease_of_Use":4.1,"Features":3.9,"Design":3.8,"Support":3.9,"Overall":3.9}</v>
+        <v>{"total_reviews":300,"ease_of_use":4.2,"features":4,"design":3.9,"support":4,"overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular IT management and monitoring tools"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Multiple tiers based on user count and features","free_version_availability":true,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"SolarWinds","Year_Founded":1999,"Country":"United States"}</v>
+        <v>{"company_name":"SolarWinds","year_founded":1999,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
+        <v>["Incident Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -748,54 +748,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":150,"Ease_of_Use":4,"Features":4.2,"Design":3.9,"Support":4,"Overall":4.1}</v>
+        <v>{"total_reviews":200,"ease_of_use":4.2,"features":4.1,"design":3.9,"support":4,"overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular IT management tools"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Contact sales for pricing information","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"TeamDynamix","Year_Founded":2001,"Country":"United States"}</v>
+        <v>{"company_name":"TeamDynamix","year_founded":2003,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","Project Management Integration"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -814,54 +814,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":200,"Ease_of_Use":4.3,"Features":4.4,"Design":4.1,"Support":4.2,"Overall":4.3}</v>
+        <v>{"total_reviews":150,"ease_of_use":4.3,"features":4.2,"design":4,"support":4.1,"overall":4.2}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular IT management tools"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Multiple tiers based on user count and features","free_version_availability":true,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"InvGate","Year_Founded":2009,"Country":"Argentina"}</v>
+        <v>{"company_name":"InvGate","year_founded":2008,"country":"Spain"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -880,54 +880,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":500,"Ease_of_Use":4.2,"Features":4.1,"Design":3.9,"Support":4,"Overall":4.1}</v>
+        <v>{"total_reviews":500,"ease_of_use":4.2,"features":4,"design":3.8,"support":4,"overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with popular monitoring and management tools"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Based on user count and features","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"SolarWinds","Year_Founded":1999,"Country":"United States"}</v>
+        <v>{"company_name":"SolarWinds","year_founded":1999,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -946,54 +946,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":400,"Ease_of_Use":4,"Features":4.2,"Design":3.8,"Support":3.9,"Overall":4}</v>
+        <v>{"total_reviews":700,"ease_of_use":4.3,"features":4.4,"design":4,"support":4.1,"overall":4.3}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with popular monitoring, security, and other business applications"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Multiple tiers based on user count and features","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"ManageEngine","Year_Founded":2001,"Country":"India"}</v>
+        <v>{"company_name":"ManageEngine","year_founded":2003,"country":"India"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1012,54 +1012,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":300,"Ease_of_Use":4.1,"Features":4.3,"Design":3.9,"Support":4,"Overall":4.1}</v>
+        <v>{"total_reviews":300,"ease_of_use":4.1,"features":4.2,"design":3.9,"support":4,"overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular IT management tools"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Multiple tiers based on user count and features","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"TOPdesk","Year_Founded":1993,"Country":"Netherlands"}</v>
+        <v>{"company_name":"TOPdesk","year_founded":1993,"country":"Netherlands"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1078,54 +1078,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":200,"Ease_of_Use":4.3,"Features":4.5,"Design":4.1,"Support":4.2,"Overall":4.4}</v>
+        <v>{"total_reviews":200,"ease_of_use":4,"features":4.3,"design":3.8,"support":3.9,"overall":4}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other IT management and business applications"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Contact sales for pricing information","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":true,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":true,"In-Person_Training":true}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"SymphonyAI","Year_Founded":2017,"Country":"United States"}</v>
+        <v>{"company_name":"SymphonyAI","year_founded":2017,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","IT Operations Management","AI-powered Chatbot","Predictive Analytics","Automation"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","AI-powered automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1144,54 +1144,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":1000,"Ease_of_Use":4.2,"Features":4.4,"Design":4,"Support":4.1,"Overall":4.3}</v>
+        <v>{"total_reviews":1200,"ease_of_use":4.4,"features":4.6,"design":4.2,"support":4.1,"overall":4.5}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":true,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular Atlassian tools and third-party applications"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Multiple tiers based on user count and features","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":true,"In-Person_Training":true}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"Atlassian","Year_Founded":2002,"Country":"Australia"}</v>
+        <v>{"company_name":"Atlassian","year_founded":2002,"country":"Australia"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","Project Management Integration"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Automation","Workflow Management","AI-powered insights"]</v>
       </c>
     </row>
   </sheetData>
@@ -1210,54 +1210,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":200,"Ease_of_Use":3.8,"Features":4,"Design":3.7,"Support":3.9,"Overall":3.8}</v>
+        <v>{"total_reviews":400,"ease_of_use":4.2,"features":4.3,"design":3.9,"support":4,"overall":4.2}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular IT management tools"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":false,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Contact sales for pricing information","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
         <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"Cherwell Software","Year_Founded":1997,"Country":"United States"}</v>
+        <v>{"company_name":"Cherwell Software","year_founded":1997,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1276,54 +1276,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":600,"Ease_of_Use":4.4,"Features":4.3,"Design":4.2,"Support":4.1,"Overall":4.3}</v>
+        <v>{"total_reviews":600,"ease_of_use":4.5,"features":4.4,"design":4.3,"support":4.2,"overall":4.5}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular CRM, IT management, and business applications"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Multiple tiers based on user count and features","free_version_availability":true,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"Freshworks","Year_Founded":2010,"Country":"India"}</v>
+        <v>{"company_name":"Freshworks","year_founded":2010,"country":"India"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","AI-powered Chatbot"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>
@@ -1342,54 +1342,54 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>Ratings</v>
+        <v>ratings</v>
       </c>
       <c r="B1" t="str">
-        <v>API_and_Integration_Support</v>
+        <v>api_and_integration_support</v>
       </c>
       <c r="C1" t="str">
-        <v>Pricing_Details</v>
+        <v>pricing_details</v>
       </c>
       <c r="D1" t="str">
-        <v>Deployment_Support</v>
+        <v>deployment_support</v>
       </c>
       <c r="E1" t="str">
-        <v>Customer_Support_Options</v>
+        <v>customer_support_options</v>
       </c>
       <c r="F1" t="str">
-        <v>Training_Platforms</v>
+        <v>training_platforms</v>
       </c>
       <c r="G1" t="str">
-        <v>Vendor_Details</v>
+        <v>vendor_details</v>
       </c>
       <c r="H1" t="str">
-        <v>List_of_Features</v>
+        <v>features</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"Total_Reviews":300,"Ease_of_Use":4,"Features":4.1,"Design":3.8,"Support":4,"Overall":4}</v>
+        <v>{"total_reviews":400,"ease_of_use":4.3,"features":4.2,"design":4,"support":4.1,"overall":4.2}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"API_Access":true,"Integration_Support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other Available Integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":false,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":false,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":"Integrations with other popular IT management and security tools"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"Pricing_Tiers":"Multiple tiers based on user count and features","Free_Version_Availability":true,"Free_Trial_Availability":true}</v>
+        <v>{"pricing_tiers":"Multiple tiers based on user count and features","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"Phone_Support":true,"24/7_Live_Support":false,"Online_Support":true}</v>
+        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
-        <v>{"Documentation":true,"Webinars":true,"Live_Online_Sessions":false,"In-Person_Training":false}</v>
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"Company_Name":"SysAid Technologies","Year_Founded":1999,"Country":"Israel"}</v>
+        <v>{"company_name":"SysAid Technologies","year_founded":1999,"country":"Israel"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Service Catalog","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","Remote Desktop Support"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Service Level Management","Knowledge Management","Asset Management","IT Service Catalog","Reporting and Analytics","Workflow Management","Basic automation"]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modification in openai prompt and settings
</commit_message>
<xml_diff>
--- a/PROJECT_features.xlsx
+++ b/PROJECT_features.xlsx
@@ -4,8 +4,20 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="ServiceNow ITSM" sheetId="1" r:id="rId1"/>
-    <sheet name="Jira Service Management" sheetId="2" r:id="rId2"/>
-    <sheet name="Freshservice" sheetId="3" r:id="rId3"/>
+    <sheet name="SolarWinds Service Desk" sheetId="2" r:id="rId2"/>
+    <sheet name="ServiceDesk Plus" sheetId="3" r:id="rId3"/>
+    <sheet name="TOPdesk" sheetId="4" r:id="rId4"/>
+    <sheet name="SymphonyAI ITSM" sheetId="5" r:id="rId5"/>
+    <sheet name="Jira Service Management" sheetId="6" r:id="rId6"/>
+    <sheet name="Cherwell Service Management" sheetId="7" r:id="rId7"/>
+    <sheet name="Freshservice" sheetId="8" r:id="rId8"/>
+    <sheet name="SysAid" sheetId="9" r:id="rId9"/>
+    <sheet name="BMC Remedy ITSM" sheetId="10" r:id="rId10"/>
+    <sheet name="Ivanti Neurons ITSM" sheetId="11" r:id="rId11"/>
+    <sheet name="EV Service Manager" sheetId="12" r:id="rId12"/>
+    <sheet name="SolarWinds Web Help Desk" sheetId="13" r:id="rId13"/>
+    <sheet name="TeamDynamix ITSM" sheetId="14" r:id="rId14"/>
+    <sheet name="InvGate Service Desk" sheetId="15" r:id="rId15"/>
   </sheets>
 </workbook>
 </file>
@@ -432,19 +444,19 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":1500,"ease_of_use":4.5,"features":4.8,"design":4.2,"support":4,"overall":4.6}</v>
+        <v>{"total_reviews":2469,"ease_of_use":4.1,"features":4.4,"design":4,"support":3.9,"overall":4.2}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":true,"BigID":true,"Cozyroc SSIS+ Suite":true,"CloudHub":true,"Elastic Observability":true,"Exalate":true,"Incydr":true,"Nexpose":true,"Other available integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":true,"assess360":true,"bigid":true,"cozyroc_ssis_suite":true,"cloudhub":true,"elastic_observability":true,"exalate":true,"incydr":true,"nexpose":true,"other_available_integrations":"Many other integrations are available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Contact sales for pricing","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":true,"online_support":true}</v>
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
         <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
@@ -453,7 +465,403 @@
         <v>{"company_name":"ServiceNow","year_founded":2004,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","IT Service Catalog","Self-service Portal","Cloud Integration"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Cloud Management","IT Operations Management","Security Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":396,"ease_of_use":3.9,"features":4.2,"design":3.8,"support":3.9,"overall":4}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Contact sales for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"BMC Software","year_founded":1980,"country":"United States"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":115,"ease_of_use":3.9,"features":4.1,"design":3.8,"support":3.9,"overall":3.9}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Contact sales for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"Ivanti","year_founded":1994,"country":"United States"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":101,"ease_of_use":4,"features":4.1,"design":3.9,"support":4,"overall":4}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Contact sales for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"EV Technologies","year_founded":1997,"country":"United Kingdom"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":322,"ease_of_use":4.2,"features":4,"design":4,"support":4.1,"overall":4.1}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Starts at $15 per user/month","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":false}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"SolarWinds","year_founded":1999,"country":"United States"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":240,"ease_of_use":4.1,"features":4.2,"design":3.9,"support":4,"overall":4.1}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Contact sales for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"TeamDynamix","year_founded":2001,"country":"United States"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":201,"ease_of_use":4.1,"features":4.2,"design":3.9,"support":4,"overall":4.1}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Starts at $10 per user/month","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":false}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"InvGate","year_founded":2010,"country":"Argentina"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -498,28 +906,28 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":1200,"ease_of_use":4.3,"features":4.6,"design":4,"support":3.8,"overall":4.4}</v>
+        <v>{"total_reviews":325,"ease_of_use":4.2,"features":4,"design":4,"support":4.1,"overall":4.1}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":true,"Elastic Observability":false,"Exalate":true,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Contact for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Starts at $15 per user/month","free_version_availability":false,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":false}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
         <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
-        <v>{"company_name":"Atlassian","year_founded":2002,"country":"Australia"}</v>
+        <v>{"company_name":"SolarWinds","year_founded":1999,"country":"United States"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","IT Service Catalog","Self-service Portal"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
       </c>
     </row>
   </sheetData>
@@ -564,28 +972,424 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>{"total_reviews":900,"ease_of_use":4.4,"features":4.2,"design":4,"support":4.1,"overall":4.3}</v>
+        <v>{"total_reviews":533,"ease_of_use":4.1,"features":4.3,"design":3.9,"support":4.2,"overall":4.2}</v>
       </c>
       <c r="B2" t="str">
-        <v>{"api_access":true,"integration_support":{"Active Directory":true,"Answer GPT":true,"Assess360":false,"BigID":false,"Cozyroc SSIS+ Suite":false,"CloudHub":true,"Elastic Observability":false,"Exalate":false,"Incydr":false,"Nexpose":false,"Other available integrations":true}}</v>
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
       </c>
       <c r="C2" t="str">
-        <v>{"pricing_tiers":"Starts at $19/agent/month","free_version_availability":true,"free_trial_availability":true}</v>
+        <v>{"pricing_tiers":"Starts at $1 per user/month","free_version_availability":true,"free_trial_availability":true}</v>
       </c>
       <c r="D2" t="str">
-        <v>{"SaaS":true,"iPhone":true,"iPad":true,"Android":true,"Windows":true,"Mac":true,"Linux":true}</v>
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
       </c>
       <c r="E2" t="str">
-        <v>{"phone_support":true,"24/7_live_support":false,"online_support":true}</v>
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
       </c>
       <c r="F2" t="str">
         <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
       </c>
       <c r="G2" t="str">
+        <v>{"company_name":"ManageEngine","year_founded":2001,"country":"India"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":294,"ease_of_use":4.1,"features":4.2,"design":3.9,"support":4,"overall":4.1}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Contact sales for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"TOPdesk","year_founded":1993,"country":"Netherlands"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":112,"ease_of_use":4,"features":4.3,"design":3.9,"support":4.1,"overall":4.2}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Contact sales for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"SymphonyAI","year_founded":2017,"country":"United States"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":2294,"ease_of_use":4.1,"features":4.3,"design":4,"support":3.9,"overall":4.2}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Starts at $7 per user/month","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"Atlassian","year_founded":2002,"country":"Australia"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":165,"ease_of_use":4,"features":4.2,"design":3.9,"support":4.1,"overall":4.1}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Contact sales for pricing","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":true}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"Cherwell Software","year_founded":1997,"country":"United States"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":1166,"ease_of_use":4.2,"features":4.3,"design":4.1,"support":4,"overall":4.2}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Starts at $19 per user/month","free_version_availability":true,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":false}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+      </c>
+      <c r="G2" t="str">
         <v>{"company_name":"Freshworks","year_founded":2010,"country":"India"}</v>
       </c>
       <c r="H2" t="str">
-        <v>["Incident Management","Problem Management","Change Management","Knowledge Management","Asset Management","Service Level Management","Reporting and Analytics","Workflow Automation","IT Service Catalog","Self-service Portal"]</v>
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
+      </c>
+    </row>
+  </sheetData>
+  <ignoredErrors>
+    <ignoredError numberStoredAsText="1" sqref="A1:H2"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>ratings</v>
+      </c>
+      <c r="B1" t="str">
+        <v>api_and_integration_support</v>
+      </c>
+      <c r="C1" t="str">
+        <v>pricing_details</v>
+      </c>
+      <c r="D1" t="str">
+        <v>deployment_support</v>
+      </c>
+      <c r="E1" t="str">
+        <v>customer_support_options</v>
+      </c>
+      <c r="F1" t="str">
+        <v>training_platforms</v>
+      </c>
+      <c r="G1" t="str">
+        <v>vendor_details</v>
+      </c>
+      <c r="H1" t="str">
+        <v>features</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>{"total_reviews":374,"ease_of_use":4,"features":4.2,"design":3.9,"support":4,"overall":4}</v>
+      </c>
+      <c r="B2" t="str">
+        <v>{"api_access":true,"integration_support":{"active_directory":true,"answer_gpt":false,"assess360":false,"bigid":false,"cozyroc_ssis_suite":false,"cloudhub":false,"elastic_observability":false,"exalate":false,"incydr":false,"nexpose":false,"other_available_integrations":"Many other integrations are available"}}</v>
+      </c>
+      <c r="C2" t="str">
+        <v>{"pricing_tiers":"Starts at $12 per user/month","free_version_availability":false,"free_trial_availability":true}</v>
+      </c>
+      <c r="D2" t="str">
+        <v>{"saas":true,"iphone":true,"ipad":true,"android":true,"windows":true,"mac":true,"linux":true}</v>
+      </c>
+      <c r="E2" t="str">
+        <v>{"phone_support":true,"live_support":true,"online_support":true}</v>
+      </c>
+      <c r="F2" t="str">
+        <v>{"documentation":true,"webinars":true,"live_online_sessions":true,"in_person_training":false}</v>
+      </c>
+      <c r="G2" t="str">
+        <v>{"company_name":"SysAid","year_founded":1999,"country":"Israel"}</v>
+      </c>
+      <c r="H2" t="str">
+        <v>["Incident Management","Problem Management","Change Management","Asset Management","Service Catalog","Knowledge Management","Reporting and Analytics","Workflow Automation","IT Service Portfolio Management","Customer Service Management"]</v>
       </c>
     </row>
   </sheetData>

</xml_diff>